<commit_message>
Update User Profile Implementation
</commit_message>
<xml_diff>
--- a/Scribbliator Technical Doc.xlsx
+++ b/Scribbliator Technical Doc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="144">
   <si>
     <t>Status</t>
   </si>
@@ -467,6 +467,27 @@
   </si>
   <si>
     <t>WebAPI</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Basic Server Routing</t>
+  </si>
+  <si>
+    <t>Able to... "Send Form Data to Server" and "Server back to Front End"</t>
+  </si>
+  <si>
+    <t>Parse Data and Insert to Database</t>
+  </si>
+  <si>
+    <t>Insert to Database, Retrieve from Database</t>
+  </si>
+  <si>
+    <t>DB Login</t>
+  </si>
+  <si>
+    <t>Change logic from Local Storage to Database</t>
   </si>
 </sst>
 </file>
@@ -726,7 +747,787 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="129">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -863,6 +1664,42 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -959,659 +1796,431 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5630,10 +6239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5642,7 +6251,7 @@
     <col min="2" max="2" width="23" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="2" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="116.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
@@ -5781,44 +6390,44 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="E10" s="11"/>
+      <c r="E10" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="E11" s="7"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="E13" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="E13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:14">
       <c r="E14" s="9" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="E15" s="10" t="s">
-        <v>104</v>
+      <c r="E15" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>105</v>
@@ -5829,53 +6438,53 @@
     </row>
     <row r="16" spans="1:14">
       <c r="E16" s="10" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="5:8">
       <c r="E17" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8">
+      <c r="E18" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8">
-      <c r="E18" s="27" t="s">
-        <v>15</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="5:8">
-      <c r="E19" s="28" t="s">
-        <v>17</v>
+      <c r="E19" s="27" t="s">
+        <v>15</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="5:8">
-      <c r="E20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>105</v>
+      <c r="E20" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="5:8">
       <c r="E21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>105</v>
@@ -5886,69 +6495,81 @@
     </row>
     <row r="22" spans="5:8">
       <c r="E22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="5:8">
-      <c r="E25" s="29" t="s">
+    <row r="23" spans="5:8">
+      <c r="E23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8">
+      <c r="E26" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+    </row>
+    <row r="27" spans="5:8">
+      <c r="E27" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8">
+      <c r="E28" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8">
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="5:8">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="5:8">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="5:8">
+      <c r="E32" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="5:8">
-      <c r="E26" s="9" t="s">
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+    </row>
+    <row r="33" spans="5:16">
+      <c r="E33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="5:8">
-      <c r="E29" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="5:8">
-      <c r="E30" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="5:16">
-      <c r="E33" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-    </row>
-    <row r="34" spans="5:16">
-      <c r="E34" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H34" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5956,11 +6577,26 @@
       <c r="P35" s="6"/>
     </row>
     <row r="36" spans="5:16">
+      <c r="E36" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="31"/>
       <c r="K36" s="5"/>
       <c r="L36" s="2"/>
       <c r="P36" s="6"/>
     </row>
     <row r="37" spans="5:16">
+      <c r="E37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K37" s="5"/>
       <c r="L37" s="2"/>
       <c r="P37" s="6"/>
@@ -5974,340 +6610,402 @@
       <c r="P39" s="6"/>
     </row>
     <row r="40" spans="5:16">
+      <c r="E40" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="31"/>
       <c r="P40" s="6"/>
     </row>
+    <row r="41" spans="5:16">
+      <c r="E41" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H35">
-    <cfRule type="cellIs" dxfId="79" priority="105" operator="equal">
+  <conditionalFormatting sqref="H2:H42">
+    <cfRule type="cellIs" dxfId="75" priority="120" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
-    <cfRule type="cellIs" dxfId="78" priority="98" operator="equal">
+  <conditionalFormatting sqref="H2:H42">
+    <cfRule type="cellIs" dxfId="74" priority="113" operator="equal">
       <formula>"Version+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="118" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
-    <cfRule type="cellIs" dxfId="76" priority="102" operator="equal">
+  <conditionalFormatting sqref="H2:H42">
+    <cfRule type="cellIs" dxfId="72" priority="117" operator="equal">
       <formula>"""Pending"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
-    <cfRule type="cellIs" dxfId="75" priority="100" operator="equal">
+  <conditionalFormatting sqref="H2:H42">
+    <cfRule type="cellIs" dxfId="71" priority="115" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26 F5:F6 F16">
-    <cfRule type="expression" dxfId="74" priority="77">
+  <conditionalFormatting sqref="F33 F5:F6 F17 F10">
+    <cfRule type="expression" dxfId="70" priority="92">
       <formula>(H5="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26 E5:E6 E16">
-    <cfRule type="expression" dxfId="73" priority="76">
+  <conditionalFormatting sqref="E33 E5:E6 E17 E10">
+    <cfRule type="expression" dxfId="69" priority="91">
       <formula>(H5="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26 G5:G6 G16">
-    <cfRule type="expression" dxfId="72" priority="75">
+  <conditionalFormatting sqref="G33 G5:G6 G17 G10">
+    <cfRule type="expression" dxfId="68" priority="90">
       <formula>(H5="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30">
-    <cfRule type="expression" dxfId="71" priority="74">
-      <formula>(H30="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="expression" dxfId="70" priority="73">
-      <formula>(H30="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="expression" dxfId="69" priority="72">
-      <formula>(H30="Complete")</formula>
+  <conditionalFormatting sqref="F37">
+    <cfRule type="expression" dxfId="67" priority="89">
+      <formula>(H37="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="expression" dxfId="66" priority="88">
+      <formula>(H37="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="expression" dxfId="65" priority="87">
+      <formula>(H37="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="68" priority="56">
+    <cfRule type="expression" dxfId="64" priority="71">
       <formula>(H8="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="67" priority="55">
+    <cfRule type="expression" dxfId="63" priority="70">
       <formula>(H8="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="66" priority="54">
+    <cfRule type="expression" dxfId="62" priority="69">
       <formula>(H8="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="65" priority="53">
+    <cfRule type="expression" dxfId="61" priority="68">
       <formula>(H9="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="64" priority="52">
+    <cfRule type="expression" dxfId="60" priority="67">
       <formula>(H9="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="63" priority="51">
+    <cfRule type="expression" dxfId="59" priority="66">
       <formula>(H9="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="62" priority="50">
-      <formula>(H13="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="61" priority="49">
-      <formula>(H13="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="60" priority="48">
-      <formula>(H13="Complete")</formula>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="expression" dxfId="58" priority="65">
+      <formula>(H14="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="57" priority="64">
+      <formula>(H14="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="expression" dxfId="56" priority="63">
+      <formula>(H14="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="55" priority="62">
+      <formula>(H16="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="54" priority="61">
+      <formula>(H16="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="expression" dxfId="53" priority="60">
+      <formula>(H16="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="59" priority="47">
+    <cfRule type="expression" dxfId="52" priority="59">
       <formula>(H15="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="58" priority="46">
+    <cfRule type="expression" dxfId="51" priority="58">
       <formula>(H15="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="expression" dxfId="57" priority="45">
+    <cfRule type="expression" dxfId="50" priority="57">
       <formula>(H15="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="56" priority="44">
-      <formula>(H14="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="55" priority="43">
-      <formula>(H14="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="expression" dxfId="54" priority="42">
-      <formula>(H14="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
-    <cfRule type="expression" dxfId="53" priority="41">
-      <formula>(H17="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="52" priority="40">
-      <formula>(H17="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="51" priority="39">
-      <formula>(H17="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="50" priority="38">
+    <cfRule type="expression" dxfId="49" priority="56">
       <formula>(H18="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="49" priority="37">
+    <cfRule type="expression" dxfId="48" priority="55">
       <formula>(H18="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="expression" dxfId="48" priority="36">
+    <cfRule type="expression" dxfId="47" priority="54">
       <formula>(H18="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="47" priority="35">
+    <cfRule type="expression" dxfId="46" priority="53">
       <formula>(H19="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="46" priority="34">
+    <cfRule type="expression" dxfId="45" priority="52">
       <formula>(H19="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="expression" dxfId="45" priority="33">
+    <cfRule type="expression" dxfId="44" priority="51">
       <formula>(H19="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="44" priority="32">
+    <cfRule type="expression" dxfId="43" priority="50">
       <formula>(H20="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="43" priority="31">
+    <cfRule type="expression" dxfId="42" priority="49">
       <formula>(H20="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="expression" dxfId="42" priority="30">
+    <cfRule type="expression" dxfId="41" priority="48">
       <formula>(H20="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="41" priority="29">
+    <cfRule type="expression" dxfId="40" priority="47">
       <formula>(H21="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="40" priority="28">
+    <cfRule type="expression" dxfId="39" priority="46">
       <formula>(H21="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="39" priority="27">
+    <cfRule type="expression" dxfId="38" priority="45">
       <formula>(H21="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="38" priority="26">
+    <cfRule type="expression" dxfId="37" priority="44">
       <formula>(H22="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="37" priority="25">
+    <cfRule type="expression" dxfId="36" priority="43">
       <formula>(H22="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="35" priority="42">
       <formula>(H22="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="expression" dxfId="35" priority="23">
-      <formula>(H20="Complete")</formula>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="expression" dxfId="34" priority="41">
+      <formula>(H23="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="expression" dxfId="33" priority="40">
+      <formula>(H23="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="expression" dxfId="32" priority="39">
+      <formula>(H23="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="34" priority="22">
+    <cfRule type="expression" dxfId="31" priority="38">
       <formula>(H21="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="expression" dxfId="30" priority="37">
+      <formula>(H22="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="33" priority="21">
+    <cfRule type="expression" dxfId="29" priority="36">
       <formula>(H7="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="32" priority="20">
+    <cfRule type="expression" dxfId="28" priority="35">
       <formula>(H7="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="31" priority="19">
+    <cfRule type="expression" dxfId="27" priority="34">
       <formula>(H7="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="expression" dxfId="30" priority="18">
+    <cfRule type="expression" dxfId="26" priority="33">
       <formula>(H4="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="29" priority="17">
+    <cfRule type="expression" dxfId="25" priority="32">
       <formula>(H4="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="expression" dxfId="28" priority="16">
+    <cfRule type="expression" dxfId="24" priority="31">
       <formula>(H4="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="27" priority="15">
+    <cfRule type="expression" dxfId="23" priority="30">
       <formula>(H3="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="26" priority="14">
+    <cfRule type="expression" dxfId="22" priority="29">
       <formula>(H3="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="expression" dxfId="25" priority="13">
+    <cfRule type="expression" dxfId="21" priority="28">
       <formula>(H3="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="20" priority="27">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="19" priority="26">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="expression" dxfId="18" priority="25">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="17" priority="24">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="16" priority="23">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="14" priority="21">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="13" priority="20">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="expression" dxfId="12" priority="19">
+      <formula>(H11="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="expression" dxfId="11" priority="18">
+      <formula>(H41="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="expression" dxfId="10" priority="17">
+      <formula>(H41="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="expression" dxfId="9" priority="16">
+      <formula>(H41="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:F31">
+    <cfRule type="expression" dxfId="8" priority="15">
+      <formula>(H27="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:E31">
+    <cfRule type="expression" dxfId="7" priority="14">
+      <formula>(H27="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:G31">
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>(H27="Complete")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="24" priority="12">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>(H10="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="23" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>(H10="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>(H10="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>(H10="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>(H10="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>(H10="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="18" priority="6">
-      <formula>(H10="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="17" priority="5">
-      <formula>(H10="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="16" priority="4">
-      <formula>(H10="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>(H34="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>(H34="Complete")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>(H34="Complete")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>